<commit_message>
fixed some errors in results
</commit_message>
<xml_diff>
--- a/data/cleaned.xlsx
+++ b/data/cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninakajdic/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\vein_ablation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7663579D-26CA-FC46-8B5D-68C46B4F22CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6541756F-E024-48E4-A8B4-B130459EC253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="210" windowWidth="36420" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="102">
   <si>
     <t>probnp</t>
   </si>
@@ -347,7 +347,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -753,86 +753,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD20976-4E45-A146-A84F-07820FEA4BED}">
   <dimension ref="A1:CP60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="AT6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BE49" sqref="BE49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="13" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" style="19" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="13" customWidth="1"/>
-    <col min="15" max="15" width="6.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="7" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" style="13" customWidth="1"/>
-    <col min="20" max="20" width="18.6640625" style="13" customWidth="1"/>
-    <col min="21" max="21" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.83203125" style="13" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="13" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" style="13" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" style="13" customWidth="1"/>
-    <col min="26" max="26" width="15.33203125" style="13" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" style="13" customWidth="1"/>
-    <col min="28" max="28" width="23.5" style="13" customWidth="1"/>
-    <col min="29" max="29" width="23.33203125" style="13" customWidth="1"/>
-    <col min="30" max="30" width="20.5" style="13" customWidth="1"/>
-    <col min="31" max="31" width="18.1640625" style="13" customWidth="1"/>
-    <col min="32" max="32" width="17.5" style="13" customWidth="1"/>
-    <col min="33" max="33" width="18.1640625" style="13" customWidth="1"/>
-    <col min="34" max="34" width="21.1640625" style="13" customWidth="1"/>
-    <col min="35" max="35" width="19.5" style="13" customWidth="1"/>
-    <col min="36" max="47" width="10.83203125" style="13"/>
-    <col min="48" max="48" width="19" style="13" customWidth="1"/>
-    <col min="49" max="49" width="16.33203125" style="13" customWidth="1"/>
-    <col min="50" max="50" width="26" style="13" customWidth="1"/>
-    <col min="51" max="51" width="18.5" style="13" customWidth="1"/>
-    <col min="52" max="52" width="19.5" style="13" customWidth="1"/>
-    <col min="53" max="53" width="24.5" style="13" customWidth="1"/>
-    <col min="54" max="54" width="28.5" style="13" customWidth="1"/>
-    <col min="55" max="55" width="25.6640625" style="13" customWidth="1"/>
-    <col min="56" max="56" width="26.1640625" style="13" customWidth="1"/>
-    <col min="57" max="57" width="22.5" style="13" customWidth="1"/>
-    <col min="58" max="58" width="23" style="13" customWidth="1"/>
-    <col min="59" max="59" width="22.5" style="13" customWidth="1"/>
-    <col min="60" max="60" width="23.33203125" style="13" customWidth="1"/>
-    <col min="61" max="61" width="22.6640625" style="13" customWidth="1"/>
-    <col min="62" max="62" width="24.83203125" style="13" customWidth="1"/>
-    <col min="63" max="63" width="20.83203125" style="13" customWidth="1"/>
-    <col min="64" max="64" width="20.33203125" style="13" customWidth="1"/>
-    <col min="65" max="65" width="20.5" style="13" customWidth="1"/>
-    <col min="66" max="66" width="20.6640625" style="13" customWidth="1"/>
-    <col min="67" max="67" width="18" style="13" customWidth="1"/>
-    <col min="68" max="68" width="17.6640625" style="13" customWidth="1"/>
-    <col min="69" max="69" width="18.1640625" style="13" customWidth="1"/>
-    <col min="70" max="70" width="19.33203125" style="13" customWidth="1"/>
-    <col min="71" max="71" width="17.6640625" style="13" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="13" customWidth="1"/>
-    <col min="73" max="74" width="18.6640625" style="13" customWidth="1"/>
-    <col min="75" max="75" width="19.83203125" style="13" customWidth="1"/>
-    <col min="76" max="76" width="19.5" style="13" customWidth="1"/>
-    <col min="77" max="77" width="17.83203125" style="13" customWidth="1"/>
-    <col min="78" max="78" width="18.5" style="13" customWidth="1"/>
-    <col min="79" max="79" width="16.83203125" style="13" customWidth="1"/>
-    <col min="80" max="80" width="18.5" style="13" customWidth="1"/>
-    <col min="81" max="81" width="16.6640625" style="13" customWidth="1"/>
-    <col min="82" max="82" width="17.33203125" style="13" customWidth="1"/>
-    <col min="83" max="16384" width="10.83203125" style="13"/>
+    <col min="20" max="20" width="18.7109375" style="13" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" style="13" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" style="13" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" style="13" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" style="13" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21" style="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" style="13" customWidth="1"/>
+    <col min="35" max="35" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="7" style="13" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6" style="13" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="27.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="25.7109375" style="13" customWidth="1"/>
+    <col min="56" max="56" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="16.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="16.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16" style="13" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="15.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="15.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="15.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="15.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="20.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="18.85546875" style="13" customWidth="1"/>
+    <col min="88" max="88" width="20.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="29.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="28.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="29" style="13" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="28.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="95" max="16384" width="10.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="156" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:94" ht="54.75" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
@@ -1116,7 +1133,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:94">
       <c r="A2" s="13" t="s">
         <v>82</v>
       </c>
@@ -1271,17 +1288,17 @@
       <c r="AZ2" s="13">
         <v>18.000000000000014</v>
       </c>
-      <c r="BA2" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB2" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC2" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="13">
-        <v>0</v>
+      <c r="BA2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD2" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE2" s="13">
         <v>1</v>
@@ -1326,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:94">
       <c r="A3" s="13" t="s">
         <v>83</v>
       </c>
@@ -1483,14 +1500,14 @@
       <c r="AZ3" s="13">
         <v>116.99999999999999</v>
       </c>
-      <c r="BA3" s="13">
-        <v>0</v>
+      <c r="BA3" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB3" s="13">
         <v>3.7166666666666668</v>
       </c>
-      <c r="BC3" s="13">
-        <v>0</v>
+      <c r="BC3" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD3" s="13">
         <v>10</v>
@@ -1610,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:94">
       <c r="A4" s="13" t="s">
         <v>82</v>
       </c>
@@ -1858,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:94">
       <c r="A5" s="13" t="s">
         <v>83</v>
       </c>
@@ -2022,8 +2039,8 @@
       <c r="BC5" s="13">
         <v>4</v>
       </c>
-      <c r="BD5" s="13">
-        <v>0</v>
+      <c r="BD5" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE5" s="13">
         <v>1</v>
@@ -2140,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:94">
       <c r="A6" s="13" t="s">
         <v>83</v>
       </c>
@@ -2295,17 +2312,17 @@
       <c r="AZ6" s="13">
         <v>65.000000000000085</v>
       </c>
-      <c r="BA6" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB6" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="13">
-        <v>0</v>
+      <c r="BA6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD6" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE6" s="13">
         <v>1</v>
@@ -2422,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:94">
       <c r="A7" s="13" t="s">
         <v>83</v>
       </c>
@@ -2579,17 +2596,17 @@
       <c r="AZ7" s="13">
         <v>85.000000000000014</v>
       </c>
-      <c r="BA7" s="13">
-        <v>0</v>
+      <c r="BA7" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB7" s="13">
         <v>6.1333333333333337</v>
       </c>
-      <c r="BC7" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD7" s="13">
-        <v>0</v>
+      <c r="BC7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD7" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE7" s="13">
         <v>1</v>
@@ -2706,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:94">
       <c r="A8" s="13" t="s">
         <v>82</v>
       </c>
@@ -2949,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:94">
       <c r="A9" s="12" t="s">
         <v>83</v>
       </c>
@@ -3104,14 +3121,14 @@
       <c r="AZ9" s="13">
         <v>80.000000000000028</v>
       </c>
-      <c r="BA9" s="13">
-        <v>0</v>
+      <c r="BA9" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB9" s="13">
         <v>7.3</v>
       </c>
-      <c r="BC9" s="13">
-        <v>0</v>
+      <c r="BC9" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD9" s="13">
         <v>19</v>
@@ -3231,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:94">
       <c r="A10" s="13" t="s">
         <v>83</v>
       </c>
@@ -3272,6 +3289,9 @@
       <c r="N10" s="13" t="s">
         <v>2</v>
       </c>
+      <c r="O10" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="P10" s="13">
         <v>0</v>
       </c>
@@ -3510,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:94">
       <c r="A11" s="13" t="s">
         <v>82</v>
       </c>
@@ -3674,8 +3694,8 @@
       <c r="BC11" s="13">
         <v>10</v>
       </c>
-      <c r="BD11" s="13">
-        <v>0</v>
+      <c r="BD11" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE11" s="13">
         <v>1</v>
@@ -3756,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:94">
       <c r="A12" s="13" t="s">
         <v>83</v>
       </c>
@@ -3911,17 +3931,17 @@
       <c r="AZ12" s="13">
         <v>46.000000000000078</v>
       </c>
-      <c r="BA12" s="13">
-        <v>0</v>
+      <c r="BA12" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB12" s="13">
         <v>1.8</v>
       </c>
-      <c r="BC12" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="13">
-        <v>0</v>
+      <c r="BC12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD12" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE12" s="13">
         <v>1</v>
@@ -4038,7 +4058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:94">
       <c r="A13" s="13" t="s">
         <v>83</v>
       </c>
@@ -4079,6 +4099,9 @@
       <c r="N13" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="O13" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="P13" s="13">
         <v>0</v>
       </c>
@@ -4190,17 +4213,17 @@
       <c r="AZ13" s="13">
         <v>39.000000000000021</v>
       </c>
-      <c r="BA13" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB13" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD13" s="13">
-        <v>0</v>
+      <c r="BA13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD13" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE13" s="13">
         <v>1</v>
@@ -4317,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:94">
       <c r="A14" s="13" t="s">
         <v>82</v>
       </c>
@@ -4358,6 +4381,9 @@
       <c r="N14" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="O14" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="P14" s="13">
         <v>0</v>
       </c>
@@ -4472,14 +4498,14 @@
       <c r="BA14" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="BB14" s="13">
-        <v>0</v>
+      <c r="BB14" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BC14" s="13">
         <v>16</v>
       </c>
-      <c r="BD14" s="13">
-        <v>0</v>
+      <c r="BD14" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE14" s="13">
         <v>1</v>
@@ -4560,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:94">
       <c r="A15" s="13" t="s">
         <v>83</v>
       </c>
@@ -4715,17 +4741,17 @@
       <c r="AZ15" s="13">
         <v>21.000000000000007</v>
       </c>
-      <c r="BA15" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB15" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC15" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD15" s="13">
-        <v>0</v>
+      <c r="BA15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD15" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE15" s="13">
         <v>1</v>
@@ -4842,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:94">
       <c r="A16" s="13" t="s">
         <v>83</v>
       </c>
@@ -5002,14 +5028,14 @@
       <c r="BA16" s="13">
         <v>5.9666666666666668</v>
       </c>
-      <c r="BB16" s="13">
-        <v>0</v>
+      <c r="BB16" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BC16" s="13">
         <v>14</v>
       </c>
-      <c r="BD16" s="13">
-        <v>0</v>
+      <c r="BD16" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE16" s="13">
         <v>1</v>
@@ -5126,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:94">
       <c r="A17" s="13" t="s">
         <v>83</v>
       </c>
@@ -5281,17 +5307,17 @@
       <c r="AZ17" s="13">
         <v>78.999999999999957</v>
       </c>
-      <c r="BA17" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB17" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC17" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD17" s="13">
-        <v>0</v>
+      <c r="BA17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD17" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE17" s="13">
         <v>1</v>
@@ -5408,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:94">
       <c r="A18" s="13" t="s">
         <v>82</v>
       </c>
@@ -5568,14 +5594,14 @@
       <c r="BA18" s="13">
         <v>5.6</v>
       </c>
-      <c r="BB18" s="13">
-        <v>0</v>
+      <c r="BB18" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BC18" s="13">
         <v>15</v>
       </c>
-      <c r="BD18" s="13">
-        <v>0</v>
+      <c r="BD18" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE18" s="13">
         <v>1</v>
@@ -5656,7 +5682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:94">
       <c r="A19" s="13" t="s">
         <v>82</v>
       </c>
@@ -5820,8 +5846,8 @@
       <c r="BC19" s="13">
         <v>8</v>
       </c>
-      <c r="BD19" s="13">
-        <v>0</v>
+      <c r="BD19" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE19" s="13">
         <v>1</v>
@@ -5902,7 +5928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:94">
       <c r="A20" s="13" t="s">
         <v>82</v>
       </c>
@@ -6062,14 +6088,14 @@
       <c r="BA20" s="13">
         <v>10.733333333333333</v>
       </c>
-      <c r="BB20" s="13">
-        <v>0</v>
+      <c r="BB20" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BC20" s="13">
         <v>27</v>
       </c>
-      <c r="BD20" s="13">
-        <v>0</v>
+      <c r="BD20" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE20" s="13">
         <v>1</v>
@@ -6150,7 +6176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:94">
       <c r="A21" s="13" t="s">
         <v>82</v>
       </c>
@@ -6307,14 +6333,14 @@
       <c r="AZ21" s="13">
         <v>80.000000000000028</v>
       </c>
-      <c r="BA21" s="13">
-        <v>0</v>
+      <c r="BA21" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB21" s="13">
         <v>2.8666666666666667</v>
       </c>
-      <c r="BC21" s="13">
-        <v>0</v>
+      <c r="BC21" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD21" s="13">
         <v>8</v>
@@ -6398,7 +6424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:94">
       <c r="A22" s="13" t="s">
         <v>82</v>
       </c>
@@ -6553,14 +6579,14 @@
       <c r="AZ22" s="13">
         <v>79.999999999999872</v>
       </c>
-      <c r="BA22" s="13">
-        <v>0</v>
+      <c r="BA22" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB22" s="13">
         <v>2.5</v>
       </c>
-      <c r="BC22" s="13">
-        <v>0</v>
+      <c r="BC22" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD22" s="13">
         <v>15</v>
@@ -6644,7 +6670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:94">
       <c r="A23" s="13" t="s">
         <v>82</v>
       </c>
@@ -6799,14 +6825,14 @@
       <c r="AZ23" s="13">
         <v>60.999999999999943</v>
       </c>
-      <c r="BA23" s="13">
-        <v>0</v>
+      <c r="BA23" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB23" s="13">
         <v>4.3833333333333346</v>
       </c>
-      <c r="BC23" s="13">
-        <v>0</v>
+      <c r="BC23" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD23" s="13">
         <v>21</v>
@@ -6890,7 +6916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:94">
       <c r="A24" s="13" t="s">
         <v>82</v>
       </c>
@@ -7045,14 +7071,14 @@
       <c r="AZ24" s="13">
         <v>109.99999999999993</v>
       </c>
-      <c r="BA24" s="13">
-        <v>0</v>
+      <c r="BA24" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB24" s="13">
         <v>2</v>
       </c>
-      <c r="BC24" s="13">
-        <v>0</v>
+      <c r="BC24" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD24" s="13">
         <v>22</v>
@@ -7136,7 +7162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:94">
       <c r="A25" s="13" t="s">
         <v>83</v>
       </c>
@@ -7291,17 +7317,17 @@
       <c r="AZ25" s="13">
         <v>43.000000000000007</v>
       </c>
-      <c r="BA25" s="13">
-        <v>0</v>
+      <c r="BA25" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB25" s="13">
         <v>2.25</v>
       </c>
-      <c r="BC25" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD25" s="13">
-        <v>0</v>
+      <c r="BC25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD25" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE25" s="13">
         <v>1</v>
@@ -7418,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:94">
       <c r="A26" s="13" t="s">
         <v>82</v>
       </c>
@@ -7666,7 +7692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:94">
       <c r="A27" s="13" t="s">
         <v>82</v>
       </c>
@@ -7912,7 +7938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:94">
       <c r="A28" s="13" t="s">
         <v>82</v>
       </c>
@@ -8067,14 +8093,14 @@
       <c r="AZ28" s="13">
         <v>52.000000000000057</v>
       </c>
-      <c r="BA28" s="13">
-        <v>0</v>
+      <c r="BA28" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB28" s="13">
         <v>1.8999999999999997</v>
       </c>
-      <c r="BC28" s="13">
-        <v>0</v>
+      <c r="BC28" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD28" s="13">
         <v>8</v>
@@ -8158,7 +8184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:94">
       <c r="A29" s="13" t="s">
         <v>82</v>
       </c>
@@ -8404,7 +8430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:94">
       <c r="A30" s="13" t="s">
         <v>82</v>
       </c>
@@ -8650,7 +8676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:94">
       <c r="A31" s="13" t="s">
         <v>82</v>
       </c>
@@ -8807,14 +8833,14 @@
       <c r="AZ31" s="13">
         <v>71.000000000000071</v>
       </c>
-      <c r="BA31" s="13">
-        <v>0</v>
+      <c r="BA31" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB31" s="13">
         <v>1.8666666666666667</v>
       </c>
-      <c r="BC31" s="13">
-        <v>0</v>
+      <c r="BC31" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD31" s="13">
         <v>7</v>
@@ -8898,7 +8924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:94">
       <c r="A32" s="13" t="s">
         <v>82</v>
       </c>
@@ -9053,14 +9079,14 @@
       <c r="AZ32" s="13">
         <v>58.000000000000036</v>
       </c>
-      <c r="BA32" s="13">
-        <v>0</v>
+      <c r="BA32" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB32" s="13">
         <v>2.8</v>
       </c>
-      <c r="BC32" s="13">
-        <v>0</v>
+      <c r="BC32" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD32" s="13">
         <v>6</v>
@@ -9144,7 +9170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:94">
       <c r="A33" s="13" t="s">
         <v>83</v>
       </c>
@@ -9301,14 +9327,14 @@
       <c r="AZ33" s="13">
         <v>140.00000000000014</v>
       </c>
-      <c r="BA33" s="13">
-        <v>0</v>
+      <c r="BA33" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB33" s="13">
         <v>5.65</v>
       </c>
-      <c r="BC33" s="13">
-        <v>0</v>
+      <c r="BC33" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD33" s="13">
         <v>11</v>
@@ -9428,7 +9454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:94">
       <c r="A34" s="13" t="s">
         <v>83</v>
       </c>
@@ -9583,17 +9609,17 @@
       <c r="AZ34" s="13">
         <v>80.999999999999957</v>
       </c>
-      <c r="BA34" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB34" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC34" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD34" s="13">
-        <v>0</v>
+      <c r="BA34" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB34" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC34" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD34" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE34" s="13">
         <v>1</v>
@@ -9710,7 +9736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:94">
       <c r="A35" s="13" t="s">
         <v>82</v>
       </c>
@@ -9865,17 +9891,17 @@
       <c r="AZ35" s="13">
         <v>72.999999999999901</v>
       </c>
-      <c r="BA35" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB35" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC35" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD35" s="13">
-        <v>0</v>
+      <c r="BA35" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB35" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC35" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD35" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE35" s="13">
         <v>1</v>
@@ -9956,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:94">
       <c r="A36" s="13" t="s">
         <v>83</v>
       </c>
@@ -10111,14 +10137,14 @@
       <c r="AZ36" s="13">
         <v>116.99999999999999</v>
       </c>
-      <c r="BA36" s="13">
-        <v>0</v>
+      <c r="BA36" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB36" s="13">
         <v>2.1666666666666665</v>
       </c>
-      <c r="BC36" s="13">
-        <v>0</v>
+      <c r="BC36" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD36" s="13">
         <v>6</v>
@@ -10238,7 +10264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:94">
       <c r="A37" s="13" t="s">
         <v>82</v>
       </c>
@@ -10395,14 +10421,14 @@
       <c r="AZ37" s="13">
         <v>106.99999999999994</v>
       </c>
-      <c r="BA37" s="13">
-        <v>0</v>
+      <c r="BA37" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB37" s="13">
         <v>4.333333333333333</v>
       </c>
-      <c r="BC37" s="13">
-        <v>0</v>
+      <c r="BC37" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD37" s="13">
         <v>15</v>
@@ -10486,7 +10512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:94">
       <c r="A38" s="13" t="s">
         <v>83</v>
       </c>
@@ -10643,17 +10669,17 @@
       <c r="AZ38" s="13">
         <v>77.000000000000043</v>
       </c>
-      <c r="BA38" s="13">
-        <v>0</v>
+      <c r="BA38" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB38" s="13">
         <v>9.8333333333333339</v>
       </c>
-      <c r="BC38" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD38" s="13">
-        <v>0</v>
+      <c r="BC38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD38" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE38" s="13">
         <v>1</v>
@@ -10770,7 +10796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:94">
       <c r="A39" s="13" t="s">
         <v>83</v>
       </c>
@@ -10927,17 +10953,17 @@
       <c r="AZ39" s="13">
         <v>123.99999999999996</v>
       </c>
-      <c r="BA39" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB39" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC39" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD39" s="13">
-        <v>0</v>
+      <c r="BA39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD39" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE39" s="13">
         <v>1</v>
@@ -11054,7 +11080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:94">
       <c r="A40" s="13" t="s">
         <v>83</v>
       </c>
@@ -11212,14 +11238,14 @@
       <c r="BA40" s="13">
         <v>3.4</v>
       </c>
-      <c r="BB40" s="13">
-        <v>0</v>
+      <c r="BB40" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BC40" s="13">
         <v>16</v>
       </c>
-      <c r="BD40" s="13">
-        <v>0</v>
+      <c r="BD40" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE40" s="13">
         <v>1</v>
@@ -11336,7 +11362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:94">
       <c r="A41" s="13" t="s">
         <v>82</v>
       </c>
@@ -11493,14 +11519,14 @@
       <c r="AZ41" s="13">
         <v>149.99999999999994</v>
       </c>
-      <c r="BA41" s="13">
-        <v>0</v>
+      <c r="BA41" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB41" s="13">
         <v>4</v>
       </c>
-      <c r="BC41" s="13">
-        <v>0</v>
+      <c r="BC41" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD41" s="13">
         <v>30</v>
@@ -11584,7 +11610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:94">
       <c r="A42" s="13" t="s">
         <v>82</v>
       </c>
@@ -11830,7 +11856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:94">
       <c r="A43" s="13" t="s">
         <v>83</v>
       </c>
@@ -11985,17 +12011,17 @@
       <c r="AZ43" s="13">
         <v>47.000000000000071</v>
       </c>
-      <c r="BA43" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB43" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC43" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD43" s="13">
-        <v>0</v>
+      <c r="BA43" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB43" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC43" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD43" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE43" s="13">
         <v>1</v>
@@ -12112,7 +12138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:94">
       <c r="A44" s="13" t="s">
         <v>83</v>
       </c>
@@ -12267,14 +12293,14 @@
       <c r="AZ44" s="13">
         <v>66</v>
       </c>
-      <c r="BA44" s="13">
-        <v>0</v>
+      <c r="BA44" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB44" s="13">
         <v>1.75</v>
       </c>
-      <c r="BC44" s="13">
-        <v>0</v>
+      <c r="BC44" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD44" s="13">
         <v>4</v>
@@ -12394,7 +12420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:94">
       <c r="A45" s="13" t="s">
         <v>82</v>
       </c>
@@ -12640,7 +12666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:94">
       <c r="A46" s="13" t="s">
         <v>82</v>
       </c>
@@ -12886,7 +12912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:94">
       <c r="A47" s="13" t="s">
         <v>83</v>
       </c>
@@ -13044,8 +13070,8 @@
       <c r="BC47" s="13">
         <v>16</v>
       </c>
-      <c r="BD47" s="13">
-        <v>0</v>
+      <c r="BD47" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE47" s="13">
         <v>1</v>
@@ -13162,7 +13188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:94">
       <c r="A48" s="13" t="s">
         <v>83</v>
       </c>
@@ -13314,17 +13340,17 @@
       <c r="AY48" s="13">
         <v>1</v>
       </c>
-      <c r="AZ48" s="13">
-        <v>0</v>
-      </c>
-      <c r="BA48" s="13">
-        <v>0</v>
+      <c r="AZ48" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA48" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB48" s="13">
         <v>6.65</v>
       </c>
-      <c r="BC48" s="13">
-        <v>0</v>
+      <c r="BC48" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD48" s="13">
         <v>17</v>
@@ -13444,7 +13470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:94">
       <c r="A49" s="13" t="s">
         <v>83</v>
       </c>
@@ -13601,17 +13627,17 @@
       <c r="AZ49" s="13">
         <v>110.00000000000009</v>
       </c>
-      <c r="BA49" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB49" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC49" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD49" s="13">
-        <v>0</v>
+      <c r="BA49" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB49" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC49" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD49" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE49" s="13">
         <v>1</v>
@@ -13728,7 +13754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:94">
       <c r="A50" s="13" t="s">
         <v>82</v>
       </c>
@@ -13883,14 +13909,14 @@
       <c r="AZ50" s="13">
         <v>56.999999999999957</v>
       </c>
-      <c r="BA50" s="13">
-        <v>0</v>
+      <c r="BA50" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB50" s="13">
         <v>3.1</v>
       </c>
-      <c r="BC50" s="13">
-        <v>0</v>
+      <c r="BC50" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD50" s="13">
         <v>13</v>
@@ -13974,7 +14000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:94">
       <c r="A51" s="13" t="s">
         <v>83</v>
       </c>
@@ -14129,17 +14155,17 @@
       <c r="AZ51" s="13">
         <v>42.000000000000014</v>
       </c>
-      <c r="BA51" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB51" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC51" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD51" s="13">
-        <v>0</v>
+      <c r="BA51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD51" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE51" s="13">
         <v>1</v>
@@ -14256,7 +14282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:94">
       <c r="A52" s="13" t="s">
         <v>83</v>
       </c>
@@ -14405,17 +14431,17 @@
       <c r="AZ52" s="13">
         <v>31.999999999999964</v>
       </c>
-      <c r="BA52" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB52" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC52" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD52" s="13">
-        <v>0</v>
+      <c r="BA52" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB52" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC52" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD52" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE52" s="13">
         <v>1</v>
@@ -14532,7 +14558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:94">
       <c r="A53" s="13" t="s">
         <v>83</v>
       </c>
@@ -14687,17 +14713,17 @@
       <c r="AZ53" s="13">
         <v>44</v>
       </c>
-      <c r="BA53" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB53" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC53" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD53" s="13">
-        <v>0</v>
+      <c r="BA53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD53" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE53" s="13">
         <v>1</v>
@@ -14814,7 +14840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:94">
       <c r="A54" s="13" t="s">
         <v>83</v>
       </c>
@@ -14969,17 +14995,17 @@
       <c r="AZ54" s="13">
         <v>62</v>
       </c>
-      <c r="BA54" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB54" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC54" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD54" s="13">
-        <v>0</v>
+      <c r="BA54" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB54" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC54" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD54" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE54" s="13">
         <v>1</v>
@@ -15096,7 +15122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:94">
       <c r="A55" s="13" t="s">
         <v>82</v>
       </c>
@@ -15344,7 +15370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:94">
       <c r="A56" s="13" t="s">
         <v>82</v>
       </c>
@@ -15501,14 +15527,14 @@
       <c r="AZ56" s="13">
         <v>54.00000000000005</v>
       </c>
-      <c r="BA56" s="13">
-        <v>0</v>
+      <c r="BA56" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB56" s="13">
         <v>4</v>
       </c>
-      <c r="BC56" s="13">
-        <v>0</v>
+      <c r="BC56" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD56" s="13">
         <v>16</v>
@@ -15592,7 +15618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:94">
       <c r="A57" s="13" t="s">
         <v>82</v>
       </c>
@@ -15747,11 +15773,17 @@
       <c r="AZ57" s="13">
         <v>52.000000000000057</v>
       </c>
+      <c r="BA57" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB57" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="BC57" s="13">
         <v>6</v>
       </c>
-      <c r="BD57" s="13">
-        <v>0</v>
+      <c r="BD57" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE57" s="13">
         <v>1</v>
@@ -15832,7 +15864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:94">
       <c r="A58" s="13" t="s">
         <v>83</v>
       </c>
@@ -15990,14 +16022,14 @@
       <c r="BA58" s="13">
         <v>1.3666666666666667</v>
       </c>
-      <c r="BB58" s="13">
-        <v>0</v>
+      <c r="BB58" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BC58" s="13">
         <v>10</v>
       </c>
-      <c r="BD58" s="13">
-        <v>0</v>
+      <c r="BD58" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE58" s="13">
         <v>1</v>
@@ -16114,7 +16146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:94">
       <c r="A59" s="13" t="s">
         <v>82</v>
       </c>
@@ -16269,14 +16301,14 @@
       <c r="AZ59" s="13">
         <v>91</v>
       </c>
-      <c r="BA59" s="13">
-        <v>0</v>
+      <c r="BA59" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BB59" s="13">
         <v>6.6</v>
       </c>
-      <c r="BC59" s="13">
-        <v>0</v>
+      <c r="BC59" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BD59" s="13">
         <v>15</v>
@@ -16360,7 +16392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:94" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:94">
       <c r="A60" s="13" t="s">
         <v>83</v>
       </c>
@@ -16515,17 +16547,17 @@
       <c r="AZ60" s="13">
         <v>27</v>
       </c>
-      <c r="BA60" s="13">
-        <v>0</v>
-      </c>
-      <c r="BB60" s="13">
-        <v>0</v>
-      </c>
-      <c r="BC60" s="13">
-        <v>0</v>
-      </c>
-      <c r="BD60" s="13">
-        <v>0</v>
+      <c r="BA60" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB60" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC60" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD60" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="BE60" s="13">
         <v>1</v>

</xml_diff>